<commit_message>
Se agregaron tablas y validaciones
Se agregaron las tablas estáticas: Institución, facultad y carrera. Se agregó validación de formato de cédula y validación de carrera
</commit_message>
<xml_diff>
--- a/uploads/studiantes.xlsx
+++ b/uploads/studiantes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\API_SC\archivos de prueba\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2118C28F-1A53-4919-9AC6-9E754A9F9633}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA3A176C-8FB3-4D0C-A126-3B58DAFB5ADA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2196" yWindow="2196" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="33">
   <si>
     <t>Nombre</t>
   </si>
@@ -47,27 +47,9 @@
     <t>Carrera</t>
   </si>
   <si>
-    <t>V-26554125</t>
-  </si>
-  <si>
-    <t>V-26554126</t>
-  </si>
-  <si>
     <t>V-26554127</t>
   </si>
   <si>
-    <t>V-26554128</t>
-  </si>
-  <si>
-    <t>V-26554129</t>
-  </si>
-  <si>
-    <t>V-26554130</t>
-  </si>
-  <si>
-    <t>V-26554131</t>
-  </si>
-  <si>
     <t>Estudiante 1</t>
   </si>
   <si>
@@ -117,6 +99,39 @@
   </si>
   <si>
     <t>Física</t>
+  </si>
+  <si>
+    <t>V26554129</t>
+  </si>
+  <si>
+    <t>v26554130</t>
+  </si>
+  <si>
+    <t>V- 26554131</t>
+  </si>
+  <si>
+    <t>EE26554126</t>
+  </si>
+  <si>
+    <t>V-265541DJNDJNJ</t>
+  </si>
+  <si>
+    <t>Biología</t>
+  </si>
+  <si>
+    <t>Estudiante 8</t>
+  </si>
+  <si>
+    <t>Apellido 8</t>
+  </si>
+  <si>
+    <t>Estudiante 9</t>
+  </si>
+  <si>
+    <t>Apellido 9</t>
+  </si>
+  <si>
+    <t>'''''''</t>
   </si>
 </sst>
 </file>
@@ -158,8 +173,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -440,10 +459,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -470,100 +489,125 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>7</v>
+      <c r="A5" s="1">
+        <v>5662332</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="D7" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D8" t="s">
-        <v>25</v>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cambios en crud de usuarios
</commit_message>
<xml_diff>
--- a/uploads/studiantes.xlsx
+++ b/uploads/studiantes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\API_SC\archivos de prueba\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA3A176C-8FB3-4D0C-A126-3B58DAFB5ADA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07751EC5-AB3F-4B3B-B811-AF1D773ABFDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2196" yWindow="2196" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="37">
   <si>
     <t>Nombre</t>
   </si>
@@ -107,9 +107,6 @@
     <t>v26554130</t>
   </si>
   <si>
-    <t>V- 26554131</t>
-  </si>
-  <si>
     <t>EE26554126</t>
   </si>
   <si>
@@ -132,13 +129,28 @@
   </si>
   <si>
     <t>'''''''</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>ffvdbdgb</t>
+  </si>
+  <si>
+    <t>Teléfono</t>
+  </si>
+  <si>
+    <t>V-26554131</t>
+  </si>
+  <si>
+    <t>Computacion</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -148,6 +160,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -173,12 +193,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -459,159 +480,220 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.88671875" customWidth="1"/>
-    <col min="2" max="2" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.109375" customWidth="1"/>
-    <col min="4" max="4" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="3" width="16.88671875" customWidth="1"/>
+    <col min="4" max="4" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.109375" customWidth="1"/>
+    <col min="6" max="6" width="23.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
       <c r="B1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2">
+        <v>22651561</v>
+      </c>
+      <c r="D2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>12</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="3">
+        <v>22651561</v>
+      </c>
+      <c r="D3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E3" t="s">
         <v>13</v>
       </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4">
+        <v>22651561</v>
+      </c>
+      <c r="D4" t="s">
         <v>7</v>
       </c>
-      <c r="C4" t="s">
+      <c r="E4" t="s">
         <v>14</v>
       </c>
-      <c r="D4" t="s">
+      <c r="F4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>5662332</v>
       </c>
       <c r="B5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5">
+        <v>22651561</v>
+      </c>
+      <c r="D5" t="s">
         <v>8</v>
       </c>
-      <c r="C5" t="s">
+      <c r="E5" t="s">
         <v>15</v>
       </c>
-      <c r="D5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>22</v>
       </c>
       <c r="B6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6">
+        <v>22651561</v>
+      </c>
+      <c r="D6" t="s">
         <v>9</v>
       </c>
-      <c r="C6" t="s">
+      <c r="E6" t="s">
         <v>16</v>
       </c>
-      <c r="D6" t="s">
+      <c r="F6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>23</v>
       </c>
       <c r="B7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7">
+        <v>22651561</v>
+      </c>
+      <c r="D7" t="s">
         <v>10</v>
       </c>
-      <c r="C7" t="s">
+      <c r="E7" t="s">
         <v>17</v>
       </c>
-      <c r="D7" t="s">
+      <c r="F7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8">
+        <v>22651561</v>
+      </c>
+      <c r="D8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9">
+        <v>22651561</v>
+      </c>
+      <c r="D9" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="E9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
-        <v>28</v>
-      </c>
-      <c r="C9" t="s">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10">
+        <v>22651561</v>
+      </c>
+      <c r="D10" t="s">
         <v>29</v>
       </c>
-      <c r="D9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10" t="s">
+      <c r="E10" t="s">
         <v>30</v>
       </c>
-      <c r="C10" t="s">
-        <v>31</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="F10" t="s">
         <v>19</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>